<commit_message>
Update WCAG article with 2.1
</commit_message>
<xml_diff>
--- a/dist/downloads/wcag02_checklist.xlsx
+++ b/dist/downloads/wcag02_checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vince\Documents\projects\devNotes\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vince\Documents\projects\devNotes\dist\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F01820-BA4D-438A-AEE0-EB938ACCA645}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC226241-B246-4104-9161-B053FBA2824D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{238E103C-CAE5-4803-8116-B188C65B1F0B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="253">
   <si>
     <t>Guideline num</t>
   </si>
@@ -635,6 +635,159 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
+  </si>
+  <si>
+    <t>Content can be display in portrait and landscape orientation</t>
+  </si>
+  <si>
+    <t>1.3.5</t>
+  </si>
+  <si>
+    <t>1.3.6</t>
+  </si>
+  <si>
+    <t>Orientation (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>1.4.10</t>
+  </si>
+  <si>
+    <t>Identify Purpose (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Reflow (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Identify Input Purpose (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>1.4.11</t>
+  </si>
+  <si>
+    <t>1.4.12</t>
+  </si>
+  <si>
+    <t>1.4.13</t>
+  </si>
+  <si>
+    <t>Non-Text Contrast  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Text Spacing  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Content on Hover or Focus  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>Character Key Shortcuts (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>2.2.6</t>
+  </si>
+  <si>
+    <t>Timeouts  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>2.3.3</t>
+  </si>
+  <si>
+    <t>Animation from Interactions  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>2.5.1</t>
+  </si>
+  <si>
+    <t>Pointer Gestures (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>2.5.2</t>
+  </si>
+  <si>
+    <t>2.5.3</t>
+  </si>
+  <si>
+    <t>2.5.4</t>
+  </si>
+  <si>
+    <t>2.5.5</t>
+  </si>
+  <si>
+    <t>2.5.6</t>
+  </si>
+  <si>
+    <t>Pointer Cancellation  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Label in Name (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Motion Actuation  (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Target Size (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>Status Messages (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Extend color contrast of at least 3:1 to non-text content such as infographics, diagrams, states, etc.</t>
+  </si>
+  <si>
+    <t>Changing text style properties shouldn't break the page (line height, spacing after paragraph, letter spacing, word spacing)</t>
+  </si>
+  <si>
+    <t>Motion animation triggered by interaction can be disabled</t>
+  </si>
+  <si>
+    <t>When using single pointer events, one of the following should be true, No Down-Event, Abort or Undo, Up Reversal, Essential</t>
+  </si>
+  <si>
+    <t>Functionalities trigger by moving the device should have a fallback without (Eg some apps use shake to undo)</t>
+  </si>
+  <si>
+    <t>The size of the target for pointer inputs is at least 44 by 44 CSS pixels</t>
+  </si>
+  <si>
+    <t>Concurrent Input Mechanisms (WCAG 2.1)</t>
+  </si>
+  <si>
+    <t>Content that is updated dynamically must be notified to users of assistive technologies without getting visual focus</t>
+  </si>
+  <si>
+    <t>Each input field must be able to be determined programmatically, a user should be able for example to autofill inputs</t>
+  </si>
+  <si>
+    <t>Interface components, icons and landmarks (sections, article, main, etc.) must be able to be identified programmatically to help navigation for assistive technologies</t>
+  </si>
+  <si>
+    <t>If using single letter keyboard shortcut, the shortcut should be able to be turn off, or remap, or active only on focus</t>
+  </si>
+  <si>
+    <t>Users should be warned if user inactivity could cause data loss, unless data is preserved for more than 20h</t>
+  </si>
+  <si>
+    <t>Complex gesture (Pinch, zooming, swiping) should have a simpler gesture alternative (Tap, double taps, long press)</t>
+  </si>
+  <si>
+    <t>Text in buttons or label should be readable by assistant technologies and can be used with Text-to-speech</t>
+  </si>
+  <si>
+    <t>User must be able to browse a website using a 320 pixel wide screen without having to scroll horizontally (There are some exceptions)</t>
+  </si>
+  <si>
+    <t>Elements that are being shown on focus or hover (skip navigation, tooltip) should be dismissible(Esc), hoverable, persistent</t>
+  </si>
+  <si>
+    <t>Inputs must to available to use with a different mechanism (Mouse, keyboard, stylus, touch, voice)</t>
   </si>
 </sst>
 </file>
@@ -724,24 +877,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -764,13 +899,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -784,6 +912,31 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -826,7 +979,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Vince" refreshedDate="43315.500483680553" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="61" xr:uid="{74A52DA1-AC4F-41B3-98D8-BC9BECF09F8D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Vince" refreshedDate="43316.765916782409" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="78" xr:uid="{74A52DA1-AC4F-41B3-98D8-BC9BECF09F8D}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table2"/>
   </cacheSource>
@@ -872,7 +1025,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="61">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="78">
   <r>
     <s v="1.1.1"/>
     <s v="Non-text Content"/>
@@ -991,6 +1144,33 @@
     <m/>
   </r>
   <r>
+    <s v="1.3.4"/>
+    <s v="Orientation (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Content can be display in portrait and landscape orientation"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="1.3.5"/>
+    <s v="Identify Input Purpose (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Each input field must be able to be determined programmatically, a user should be able for example to autofill inputs"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="1.3.6"/>
+    <s v="Identify Purpose (WCAG 2.1)"/>
+    <x v="2"/>
+    <s v="Interface components, icons and landmarks (sections, article, main, etc.) must be able to be identified programmatically to help navigation for assistive technologies"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="1.4.1"/>
     <s v="Use of Colour"/>
     <x v="0"/>
@@ -1072,6 +1252,42 @@
     <m/>
   </r>
   <r>
+    <s v="1.4.10"/>
+    <s v="Reflow (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="User must be able to browse a website using a 320 pixel wide screen without having to scroll horizontally (There are some exceptions)"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="1.4.11"/>
+    <s v="Non-Text Contrast  (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Extend color contrast of at least 3:1 to non-text content such as infographics, diagrams, states, etc."/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="1.4.12"/>
+    <s v="Text Spacing  (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Changing text style properties shouldn't break the page (line height, spacing after paragraph, letter spacing, word spacing)"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="1.4.13"/>
+    <s v="Content on Hover or Focus  (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Elements that are being shown on focus or hover (skip navigation, tooltip) should be dismissible(Esc), hoverable, persistent"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="2.1.1"/>
     <s v="Keyboard"/>
     <x v="0"/>
@@ -1099,6 +1315,15 @@
     <m/>
   </r>
   <r>
+    <s v="2.1.4"/>
+    <s v="Character Key Shortcuts (WCAG 2.1)"/>
+    <x v="0"/>
+    <s v="If using single letter keyboard shortcut, the shortcut should be able to be turn off, or remap, or active only on focus"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="2.2.1"/>
     <s v="Timing Adjustable"/>
     <x v="0"/>
@@ -1144,6 +1369,15 @@
     <m/>
   </r>
   <r>
+    <s v="2.2.6"/>
+    <s v="Timeouts  (WCAG 2.1)"/>
+    <x v="2"/>
+    <s v="Users should be warned if user inactivity could cause data loss, unless data is preserved for more than 20h"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="2.3.1"/>
     <s v="Three Flashes or Below"/>
     <x v="0"/>
@@ -1162,6 +1396,15 @@
     <m/>
   </r>
   <r>
+    <s v="2.3.3"/>
+    <s v="Animation from Interactions  (WCAG 2.1)"/>
+    <x v="2"/>
+    <s v="Motion animation triggered by interaction can be disabled"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="2.4.1"/>
     <s v="Bypass Blocks"/>
     <x v="0"/>
@@ -1252,6 +1495,60 @@
     <m/>
   </r>
   <r>
+    <s v="2.5.1"/>
+    <s v="Pointer Gestures (WCAG 2.1)"/>
+    <x v="0"/>
+    <s v="Complex gesture (Pinch, zooming, swiping) should have a simpler gesture alternative (Tap, double taps, long press)"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="2.5.2"/>
+    <s v="Pointer Cancellation  (WCAG 2.1)"/>
+    <x v="0"/>
+    <s v="When using single pointer events, one of the following should be true, No Down-Event, Abort or Undo, Up Reversal, Essential"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="2.5.3"/>
+    <s v="Label in Name (WCAG 2.1)"/>
+    <x v="0"/>
+    <s v="Text in buttons or label should be readable by assistant technologies and can be used with Text-to-speech"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="2.5.4"/>
+    <s v="Motion Actuation  (WCAG 2.1)"/>
+    <x v="0"/>
+    <s v="Functionalities trigger by moving the device should have a fallback without (Eg some apps use shake to undo)"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="2.5.5"/>
+    <s v="Target Size (WCAG 2.1)"/>
+    <x v="2"/>
+    <s v="The size of the target for pointer inputs is at least 44 by 44 CSS pixels"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="2.5.6"/>
+    <s v="Concurrent Input Mechanisms (WCAG 2.1)"/>
+    <x v="2"/>
+    <s v="Inputs must to available to use with a different mechanism (Mouse, keyboard, stylus, touch, voice)"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <s v="3.1.1"/>
     <s v="Language of Page"/>
     <x v="0"/>
@@ -1418,6 +1715,15 @@
     <s v="Name, Role, Value"/>
     <x v="0"/>
     <s v="Build all elements for accessibility"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="4.1.3"/>
+    <s v="Status Messages (WCAG 2.1)"/>
+    <x v="1"/>
+    <s v="Content that is updated dynamically must be notified to users of assistive technologies without getting visual focus"/>
     <x v="0"/>
     <m/>
     <m/>
@@ -1514,10 +1820,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CDFF02E-E859-4F4C-AF05-069548CAD3E9}" name="Table2" displayName="Table2" ref="A1:G62" totalsRowShown="0">
-  <autoFilter ref="A1:G62" xr:uid="{52480724-36BA-496E-B258-3ECAB635BC03}"/>
-  <sortState ref="A2:G62">
-    <sortCondition ref="A1:A62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CDFF02E-E859-4F4C-AF05-069548CAD3E9}" name="Table2" displayName="Table2" ref="A1:G79" totalsRowShown="0">
+  <autoFilter ref="A1:G79" xr:uid="{52480724-36BA-496E-B258-3ECAB635BC03}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G78">
+    <sortCondition ref="A1:A78"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B9B4F09D-323F-4898-93AB-733C803E0EE2}" name="Guideline num"/>
@@ -1533,10 +1839,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8576292C-5106-4F66-8CAE-BEF137EA596A}" name="Table1" displayName="Table1" ref="J1:J4" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8576292C-5106-4F66-8CAE-BEF137EA596A}" name="Table1" displayName="Table1" ref="J1:J4" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="J1:J4" xr:uid="{0CCE1151-C70E-4CF3-92B1-C5B8F1597781}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0A6FBB2F-D71A-4C92-8994-4A7DBA473F07}" name="Status" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0A6FBB2F-D71A-4C92-8994-4A7DBA473F07}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1842,7 +2148,7 @@
   <dimension ref="A3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,25 +2226,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C6" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="E6" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="G6" s="3">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H6" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="I6" s="3">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1949,25 +2255,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="E7" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F7" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="G7" s="3">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H7" s="4" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="I7" s="3">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1986,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C512F443-9E2F-4827-AA3D-1D6AFFB57A28}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D79" sqref="A1:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,7 +2303,7 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="150.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -2223,674 +2529,912 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>209</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>211</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
         <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
         <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="B43" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="C43" t="s">
         <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
         <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D53" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>248</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>230</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
       </c>
       <c r="D55" t="s">
-        <v>24</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>231</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
       </c>
       <c r="D56" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>142</v>
+        <v>227</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>232</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>228</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>233</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>229</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="C59" t="s">
         <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" t="s">
+        <v>177</v>
+      </c>
+      <c r="C62" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>178</v>
+      </c>
+      <c r="B63" t="s">
+        <v>179</v>
+      </c>
+      <c r="C63" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>29</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" t="s">
+        <v>67</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" t="s">
+        <v>187</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>118</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B78" t="s">
         <v>119</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C78" t="s">
         <v>29</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D78" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>